<commit_message>
Ajustes da versão final:
- Criptografia da base de dados;
- Inclusão de dados fictícios para teste;
- Inclusão de documentação em PDF;
</commit_message>
<xml_diff>
--- a/dados/modelo_dw.xlsx
+++ b/dados/modelo_dw.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="420" windowWidth="17955" windowHeight="11295" tabRatio="787" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="720" yWindow="420" windowWidth="17955" windowHeight="11295" tabRatio="817" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="BI_PessoaSaude" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="BI_PessoaFisicaCompleto" sheetId="5" r:id="rId3"/>
     <sheet name="BI_PessoaEducacao" sheetId="8" r:id="rId4"/>
     <sheet name="BI_PessoaVinculoInscricaoCadast" sheetId="6" r:id="rId5"/>
-    <sheet name="Plan1" sheetId="9" r:id="rId6"/>
+    <sheet name="BI_DadosInscricaoImobiliaria" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="45">
   <si>
     <t>fonte</t>
   </si>
@@ -126,82 +126,22 @@
     <t>estado</t>
   </si>
   <si>
-    <t>tipoCadastro</t>
-  </si>
-  <si>
-    <t>temDebitoDA2018</t>
-  </si>
-  <si>
-    <t>pgDebitoDA2018</t>
-  </si>
-  <si>
-    <t>temDebitoDA2019</t>
-  </si>
-  <si>
-    <t>pgDebitoDA2019</t>
-  </si>
-  <si>
-    <t>temDebitoDA2020</t>
-  </si>
-  <si>
-    <t>pgDebitoDA2020</t>
-  </si>
-  <si>
-    <t>temDebitoDA2021</t>
-  </si>
-  <si>
-    <t>pgDebitoDA2021</t>
-  </si>
-  <si>
-    <t>temDebitoDA2022</t>
-  </si>
-  <si>
-    <t>pgDebitoDA2022</t>
-  </si>
-  <si>
     <t>vlDebitoDA</t>
   </si>
   <si>
     <t>vlIPTU</t>
   </si>
   <si>
-    <t>temDebitoInscricao</t>
-  </si>
-  <si>
     <t>cpfCnpjResponsavel</t>
   </si>
   <si>
-    <t>temDebitoResponsavel</t>
-  </si>
-  <si>
-    <t>dtProcessamento</t>
-  </si>
-  <si>
     <t>nomeBairro</t>
   </si>
   <si>
     <t>nomeLogradouro</t>
   </si>
   <si>
-    <t>temItbi</t>
-  </si>
-  <si>
-    <t>temMatriculaCartorio</t>
-  </si>
-  <si>
-    <t>tipoPessoaResponsavel</t>
-  </si>
-  <si>
     <t>vlVenalImovel</t>
-  </si>
-  <si>
-    <t>dtVerificaDebito</t>
-  </si>
-  <si>
-    <t>EimoveldaPMV</t>
-  </si>
-  <si>
-    <t>temIsencaoImunidadeIPTU</t>
   </si>
   <si>
     <t>tipoIsencaoImunidadeIPTU</t>
@@ -935,28 +875,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="22.140625" bestFit="1" customWidth="1"/>
@@ -976,102 +914,48 @@
     <col min="32" max="32" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" t="s">
-        <v>41</v>
       </c>
       <c r="I1" t="s">
         <v>42</v>
       </c>
       <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
         <v>43</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>44</v>
       </c>
-      <c r="L1" t="s">
-        <v>45</v>
-      </c>
       <c r="M1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="N1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>50</v>
-      </c>
-      <c r="R1" t="s">
-        <v>51</v>
-      </c>
-      <c r="S1" t="s">
-        <v>52</v>
-      </c>
-      <c r="T1" t="s">
-        <v>53</v>
-      </c>
-      <c r="U1" t="s">
-        <v>5</v>
-      </c>
-      <c r="V1" t="s">
-        <v>54</v>
-      </c>
-      <c r="W1" t="s">
-        <v>55</v>
-      </c>
-      <c r="X1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>